<commit_message>
integration test vouchers done pass
</commit_message>
<xml_diff>
--- a/src/test/java/integrationtest/voucher/VouchersIntegrationTestData.xlsx
+++ b/src/test/java/integrationtest/voucher/VouchersIntegrationTestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/integrationtest/voucher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C91B5D-B692-6B48-9065-DE862A57EA47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0757DE11-55AD-6C4C-9EA3-4E169688480B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Voucher Promotion" sheetId="2" r:id="rId1"/>
     <sheet name="My Voucher" sheetId="3" r:id="rId2"/>
-    <sheet name="Voucher Details" sheetId="4" r:id="rId3"/>
+    <sheet name="Voucher Recommendation" sheetId="5" r:id="rId3"/>
+    <sheet name="Voucher Details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>testCase</t>
   </si>
@@ -92,6 +93,24 @@
   </si>
   <si>
     <t>Valid ID 2</t>
+  </si>
+  <si>
+    <t>transactionId</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Valid parameters</t>
+  </si>
+  <si>
+    <t>Have no vouchers</t>
+  </si>
+  <si>
+    <t>{"id":4,"name":"Cashback Rp 2.500 buat beli pulsa","voucherTypeName":"cashback","discount":0,"maxDeduction":0,"value":2500,"filePath":"https://res.cloudinary.com/darwmcfjo/image/upload/v1591548482/WhatsApp_Image_2020-05-30_at_7.27.48_PM_nessez.jpg","expiryDate":1279584000000}</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -501,7 +520,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9DB414-D404-9B43-88E0-9E486045AF39}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,16 +644,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2F92C8-0217-FD43-89A6-8508CEEAA2CB}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="254.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3261EE52-DDC4-DE48-8110-151674ED6ABC}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.6640625" customWidth="1"/>
   </cols>

</xml_diff>